<commit_message>
1.fix bug when reset value is hex;
</commit_message>
<xml_diff>
--- a/Python/reg_map/CFG.xlsx
+++ b/Python/reg_map/CFG.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\working\script\Python\reg_map\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\working\script\Python\reg_map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2720469C-D404-4478-9168-40C3C9646C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C02428B8-71E1-408E-A24B-D2A86D6897D4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="5" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="150">
   <si>
     <t>Base
 Address</t>
@@ -581,13 +580,21 @@
   </si>
   <si>
     <t>d1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hf</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -786,34 +793,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -824,6 +807,30 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1237,12 +1244,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16F4388A-EDAE-4106-B0AC-902BB21D3C4B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K77" sqref="K77"/>
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1256,49 +1263,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="14" t="s">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="14" t="s">
+      <c r="D1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="15" t="s">
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="I1" s="16"/>
-      <c r="J1" s="14" t="s">
+      <c r="I1" s="21"/>
+      <c r="J1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="14"/>
-      <c r="M1" s="18" t="s">
+      <c r="L1" s="17"/>
+      <c r="M1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="18" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="7" t="s">
         <v>10</v>
       </c>
@@ -1314,25 +1321,25 @@
       <c r="I2" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="J2" s="14"/>
+      <c r="J2" s="17"/>
       <c r="K2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="19"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="10"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="18"/>
     </row>
     <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="19" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="1">
@@ -1358,7 +1365,7 @@
       <c r="J3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="19" t="s">
         <v>19</v>
       </c>
       <c r="L3" s="1" t="s">
@@ -1371,9 +1378,9 @@
       <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
       <c r="D4" s="1"/>
       <c r="E4" s="6">
         <v>30</v>
@@ -1395,7 +1402,7 @@
       <c r="J4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="17"/>
+      <c r="K4" s="19"/>
       <c r="L4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1406,9 +1413,9 @@
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="1"/>
       <c r="E5" s="6">
         <v>27</v>
@@ -1430,7 +1437,7 @@
       <c r="J5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="17"/>
+      <c r="K5" s="19"/>
       <c r="L5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1441,9 +1448,9 @@
       <c r="O5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="1"/>
       <c r="E6" s="6">
         <v>26</v>
@@ -1465,7 +1472,7 @@
       <c r="J6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="17"/>
+      <c r="K6" s="19"/>
       <c r="L6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1476,9 +1483,9 @@
       <c r="O6" s="2"/>
     </row>
     <row r="7" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="1"/>
       <c r="E7" s="6">
         <v>23</v>
@@ -1500,7 +1507,7 @@
       <c r="J7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K7" s="17"/>
+      <c r="K7" s="19"/>
       <c r="L7" s="1" t="s">
         <v>29</v>
       </c>
@@ -1511,9 +1518,9 @@
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="1"/>
       <c r="E8" s="6">
         <v>22</v>
@@ -1535,7 +1542,7 @@
       <c r="J8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="17"/>
+      <c r="K8" s="19"/>
       <c r="L8" s="1" t="s">
         <v>29</v>
       </c>
@@ -1546,9 +1553,9 @@
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="1"/>
       <c r="E9" s="6">
         <v>19</v>
@@ -1570,7 +1577,7 @@
       <c r="J9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K9" s="17"/>
+      <c r="K9" s="19"/>
       <c r="L9" s="1" t="s">
         <v>33</v>
       </c>
@@ -1581,9 +1588,9 @@
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="1"/>
       <c r="E10" s="6">
         <v>18</v>
@@ -1605,7 +1612,7 @@
       <c r="J10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K10" s="17"/>
+      <c r="K10" s="19"/>
       <c r="L10" s="1" t="s">
         <v>33</v>
       </c>
@@ -1616,9 +1623,9 @@
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="1"/>
       <c r="E11" s="6">
         <v>15</v>
@@ -1640,7 +1647,7 @@
       <c r="J11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="17"/>
+      <c r="K11" s="19"/>
       <c r="L11" s="1" t="s">
         <v>37</v>
       </c>
@@ -1651,9 +1658,9 @@
       <c r="O11" s="2"/>
     </row>
     <row r="12" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="1"/>
       <c r="E12" s="6">
         <v>14</v>
@@ -1675,7 +1682,7 @@
       <c r="J12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K12" s="17"/>
+      <c r="K12" s="19"/>
       <c r="L12" s="1" t="s">
         <v>37</v>
       </c>
@@ -1686,9 +1693,9 @@
       <c r="O12" s="2"/>
     </row>
     <row r="13" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="1"/>
       <c r="E13" s="6">
         <v>11</v>
@@ -1710,7 +1717,7 @@
       <c r="J13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K13" s="17"/>
+      <c r="K13" s="19"/>
       <c r="L13" s="1" t="s">
         <v>40</v>
       </c>
@@ -1721,9 +1728,9 @@
       <c r="O13" s="2"/>
     </row>
     <row r="14" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="1"/>
       <c r="E14" s="6">
         <v>10</v>
@@ -1745,7 +1752,7 @@
       <c r="J14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K14" s="17"/>
+      <c r="K14" s="19"/>
       <c r="L14" s="1" t="s">
         <v>40</v>
       </c>
@@ -1756,9 +1763,9 @@
       <c r="O14" s="2"/>
     </row>
     <row r="15" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="1"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6">
@@ -1778,7 +1785,7 @@
       <c r="J15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K15" s="17"/>
+      <c r="K15" s="19"/>
       <c r="L15" s="1" t="s">
         <v>43</v>
       </c>
@@ -1789,9 +1796,9 @@
       <c r="O15" s="2"/>
     </row>
     <row r="16" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="1"/>
       <c r="E16" s="6">
         <v>6</v>
@@ -1813,7 +1820,7 @@
       <c r="J16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K16" s="17"/>
+      <c r="K16" s="19"/>
       <c r="L16" s="1" t="s">
         <v>43</v>
       </c>
@@ -1824,9 +1831,9 @@
       <c r="O16" s="2"/>
     </row>
     <row r="17" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="1"/>
       <c r="E17" s="6">
         <v>3</v>
@@ -1846,7 +1853,7 @@
       <c r="J17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K17" s="17"/>
+      <c r="K17" s="19"/>
       <c r="L17" s="1" t="s">
         <v>46</v>
       </c>
@@ -1857,9 +1864,9 @@
       <c r="O17" s="2"/>
     </row>
     <row r="18" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
       <c r="D18" s="1"/>
       <c r="E18" s="6">
         <v>2</v>
@@ -1881,7 +1888,7 @@
       <c r="J18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K18" s="17"/>
+      <c r="K18" s="19"/>
       <c r="L18" s="1" t="s">
         <v>46</v>
       </c>
@@ -1892,11 +1899,11 @@
       <c r="O18" s="2"/>
     </row>
     <row r="19" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17" t="s">
+      <c r="A19" s="19"/>
+      <c r="B19" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="19" t="s">
         <v>49</v>
       </c>
       <c r="D19" s="1"/>
@@ -1918,7 +1925,7 @@
       <c r="J19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K19" s="17" t="s">
+      <c r="K19" s="19" t="s">
         <v>19</v>
       </c>
       <c r="L19" s="1" t="s">
@@ -1931,9 +1938,9 @@
       <c r="O19" s="2"/>
     </row>
     <row r="20" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="1"/>
       <c r="E20" s="6">
         <v>30</v>
@@ -1955,7 +1962,7 @@
       <c r="J20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="K20" s="17"/>
+      <c r="K20" s="19"/>
       <c r="L20" s="1" t="s">
         <v>51</v>
       </c>
@@ -1966,9 +1973,9 @@
       <c r="O20" s="2"/>
     </row>
     <row r="21" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="1"/>
       <c r="E21" s="6">
         <v>27</v>
@@ -1990,7 +1997,7 @@
       <c r="J21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K21" s="17"/>
+      <c r="K21" s="19"/>
       <c r="L21" s="1" t="s">
         <v>54</v>
       </c>
@@ -2001,9 +2008,9 @@
       <c r="O21" s="2"/>
     </row>
     <row r="22" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
       <c r="D22" s="1"/>
       <c r="E22" s="6">
         <v>26</v>
@@ -2025,7 +2032,7 @@
       <c r="J22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="K22" s="17"/>
+      <c r="K22" s="19"/>
       <c r="L22" s="1" t="s">
         <v>54</v>
       </c>
@@ -2036,13 +2043,13 @@
       <c r="O22" s="2"/>
     </row>
     <row r="23" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>59</v>
       </c>
       <c r="D23" s="1"/>
@@ -2064,7 +2071,7 @@
       <c r="J23" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K23" s="11" t="s">
+      <c r="K23" s="10" t="s">
         <v>19</v>
       </c>
       <c r="L23" s="1" t="s">
@@ -2079,9 +2086,9 @@
       <c r="O23" s="2"/>
     </row>
     <row r="24" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
       <c r="D24" s="1"/>
       <c r="E24" s="6">
         <v>27</v>
@@ -2103,7 +2110,7 @@
       <c r="J24" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K24" s="12"/>
+      <c r="K24" s="11"/>
       <c r="L24" s="1" t="s">
         <v>61</v>
       </c>
@@ -2116,9 +2123,9 @@
       <c r="O24" s="2"/>
     </row>
     <row r="25" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
       <c r="D25" s="1"/>
       <c r="E25" s="6">
         <v>25</v>
@@ -2138,7 +2145,7 @@
       <c r="J25" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K25" s="12"/>
+      <c r="K25" s="11"/>
       <c r="L25" s="1" t="s">
         <v>64</v>
       </c>
@@ -2151,9 +2158,9 @@
       <c r="O25" s="2"/>
     </row>
     <row r="26" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
       <c r="D26" s="2"/>
       <c r="E26" s="6">
         <v>24</v>
@@ -2175,7 +2182,7 @@
       <c r="J26" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K26" s="12"/>
+      <c r="K26" s="11"/>
       <c r="L26" s="1" t="s">
         <v>64</v>
       </c>
@@ -2188,9 +2195,9 @@
       <c r="O26" s="2"/>
     </row>
     <row r="27" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
       <c r="D27" s="2"/>
       <c r="E27" s="6">
         <v>21</v>
@@ -2210,7 +2217,7 @@
       <c r="J27" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K27" s="12"/>
+      <c r="K27" s="11"/>
       <c r="L27" s="1" t="s">
         <v>67</v>
       </c>
@@ -2223,9 +2230,9 @@
       <c r="O27" s="2"/>
     </row>
     <row r="28" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
       <c r="D28" s="2"/>
       <c r="E28" s="6">
         <v>20</v>
@@ -2247,7 +2254,7 @@
       <c r="J28" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K28" s="12"/>
+      <c r="K28" s="11"/>
       <c r="L28" s="1" t="s">
         <v>67</v>
       </c>
@@ -2260,9 +2267,9 @@
       <c r="O28" s="2"/>
     </row>
     <row r="29" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
       <c r="D29" s="2"/>
       <c r="E29" s="6">
         <v>13</v>
@@ -2282,7 +2289,7 @@
       <c r="J29" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="K29" s="12"/>
+      <c r="K29" s="11"/>
       <c r="L29" s="1" t="s">
         <v>70</v>
       </c>
@@ -2295,9 +2302,9 @@
       <c r="O29" s="2"/>
     </row>
     <row r="30" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
       <c r="D30" s="2"/>
       <c r="E30" s="6">
         <v>12</v>
@@ -2319,22 +2326,22 @@
       <c r="J30" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="K30" s="12"/>
+      <c r="K30" s="11"/>
       <c r="L30" s="1" t="s">
         <v>70</v>
       </c>
       <c r="M30" s="1">
         <v>1</v>
       </c>
-      <c r="N30" s="1">
-        <v>3</v>
+      <c r="N30" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="O30" s="2"/>
     </row>
     <row r="31" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
       <c r="D31" s="2"/>
       <c r="E31" s="6">
         <v>9</v>
@@ -2354,22 +2361,22 @@
       <c r="J31" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K31" s="12"/>
+      <c r="K31" s="11"/>
       <c r="L31" s="1" t="s">
         <v>73</v>
       </c>
       <c r="M31" s="1">
         <v>1</v>
       </c>
-      <c r="N31" s="1">
-        <v>1</v>
+      <c r="N31" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="O31" s="2"/>
     </row>
     <row r="32" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
       <c r="D32" s="2"/>
       <c r="E32" s="6">
         <v>8</v>
@@ -2391,7 +2398,7 @@
       <c r="J32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K32" s="12"/>
+      <c r="K32" s="11"/>
       <c r="L32" s="1" t="s">
         <v>73</v>
       </c>
@@ -2404,9 +2411,9 @@
       <c r="O32" s="2"/>
     </row>
     <row r="33" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
       <c r="D33" s="2"/>
       <c r="E33" s="6">
         <v>5</v>
@@ -2426,7 +2433,7 @@
       <c r="J33" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="K33" s="12"/>
+      <c r="K33" s="11"/>
       <c r="L33" s="1" t="s">
         <v>76</v>
       </c>
@@ -2439,9 +2446,9 @@
       <c r="O33" s="2"/>
     </row>
     <row r="34" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
       <c r="D34" s="2"/>
       <c r="E34" s="6">
         <v>4</v>
@@ -2463,7 +2470,7 @@
       <c r="J34" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="K34" s="20"/>
+      <c r="K34" s="12"/>
       <c r="L34" s="1" t="s">
         <v>76</v>
       </c>
@@ -2476,13 +2483,13 @@
       <c r="O34" s="2"/>
     </row>
     <row r="35" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="10" t="s">
         <v>80</v>
       </c>
       <c r="D35" s="2"/>
@@ -2504,7 +2511,7 @@
       <c r="J35" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K35" s="11" t="s">
+      <c r="K35" s="10" t="s">
         <v>19</v>
       </c>
       <c r="L35" s="1" t="s">
@@ -2519,9 +2526,9 @@
       <c r="O35" s="2"/>
     </row>
     <row r="36" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
+      <c r="A36" s="14"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
       <c r="D36" s="2"/>
       <c r="E36" s="6">
         <v>29</v>
@@ -2543,7 +2550,7 @@
       <c r="J36" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="K36" s="12"/>
+      <c r="K36" s="11"/>
       <c r="L36" s="1" t="s">
         <v>82</v>
       </c>
@@ -2556,9 +2563,9 @@
       <c r="O36" s="2"/>
     </row>
     <row r="37" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
+      <c r="A37" s="14"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
       <c r="D37" s="2"/>
       <c r="E37" s="6">
         <v>14</v>
@@ -2578,7 +2585,7 @@
       <c r="J37" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K37" s="12"/>
+      <c r="K37" s="11"/>
       <c r="L37" s="1" t="s">
         <v>85</v>
       </c>
@@ -2591,9 +2598,9 @@
       <c r="O37" s="2"/>
     </row>
     <row r="38" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
+      <c r="A38" s="14"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
       <c r="D38" s="2"/>
       <c r="E38" s="6">
         <v>13</v>
@@ -2615,7 +2622,7 @@
       <c r="J38" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K38" s="12"/>
+      <c r="K38" s="11"/>
       <c r="L38" s="1" t="s">
         <v>85</v>
       </c>
@@ -2628,9 +2635,9 @@
       <c r="O38" s="2"/>
     </row>
     <row r="39" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
+      <c r="A39" s="14"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
       <c r="D39" s="2"/>
       <c r="E39" s="6">
         <v>10</v>
@@ -2650,7 +2657,7 @@
       <c r="J39" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K39" s="12"/>
+      <c r="K39" s="11"/>
       <c r="L39" s="1" t="s">
         <v>88</v>
       </c>
@@ -2663,9 +2670,9 @@
       <c r="O39" s="2"/>
     </row>
     <row r="40" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
+      <c r="A40" s="14"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
       <c r="D40" s="2"/>
       <c r="E40" s="6">
         <v>7</v>
@@ -2687,7 +2694,7 @@
       <c r="J40" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="K40" s="12"/>
+      <c r="K40" s="11"/>
       <c r="L40" s="1" t="s">
         <v>88</v>
       </c>
@@ -2700,9 +2707,9 @@
       <c r="O40" s="2"/>
     </row>
     <row r="41" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
       <c r="D41" s="2"/>
       <c r="E41" s="6">
         <v>5</v>
@@ -2722,7 +2729,7 @@
       <c r="J41" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K41" s="12"/>
+      <c r="K41" s="11"/>
       <c r="L41" s="1" t="s">
         <v>91</v>
       </c>
@@ -2735,9 +2742,9 @@
       <c r="O41" s="2"/>
     </row>
     <row r="42" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
+      <c r="A42" s="14"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
       <c r="D42" s="2"/>
       <c r="E42" s="6">
         <v>4</v>
@@ -2759,7 +2766,7 @@
       <c r="J42" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K42" s="12"/>
+      <c r="K42" s="11"/>
       <c r="L42" s="1" t="s">
         <v>91</v>
       </c>
@@ -2772,9 +2779,9 @@
       <c r="O42" s="2"/>
     </row>
     <row r="43" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
+      <c r="A43" s="14"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
       <c r="D43" s="2"/>
       <c r="E43" s="6">
         <v>2</v>
@@ -2794,7 +2801,7 @@
       <c r="J43" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K43" s="12"/>
+      <c r="K43" s="11"/>
       <c r="L43" s="1" t="s">
         <v>94</v>
       </c>
@@ -2807,9 +2814,9 @@
       <c r="O43" s="2"/>
     </row>
     <row r="44" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
+      <c r="A44" s="14"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
       <c r="D44" s="2"/>
       <c r="E44" s="6">
         <v>1</v>
@@ -2831,7 +2838,7 @@
       <c r="J44" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="K44" s="20"/>
+      <c r="K44" s="12"/>
       <c r="L44" s="1" t="s">
         <v>94</v>
       </c>
@@ -2844,11 +2851,11 @@
       <c r="O44" s="2"/>
     </row>
     <row r="45" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
-      <c r="B45" s="11" t="s">
+      <c r="A45" s="14"/>
+      <c r="B45" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="10" t="s">
         <v>97</v>
       </c>
       <c r="D45" s="3"/>
@@ -2870,7 +2877,7 @@
       <c r="J45" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="K45" s="11" t="s">
+      <c r="K45" s="10" t="s">
         <v>19</v>
       </c>
       <c r="L45" s="1" t="s">
@@ -2885,9 +2892,9 @@
       <c r="O45" s="2"/>
     </row>
     <row r="46" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
+      <c r="A46" s="14"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
       <c r="D46" s="3"/>
       <c r="E46" s="6">
         <v>25</v>
@@ -2909,7 +2916,7 @@
       <c r="J46" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K46" s="12"/>
+      <c r="K46" s="11"/>
       <c r="L46" s="1" t="s">
         <v>99</v>
       </c>
@@ -2922,9 +2929,9 @@
       <c r="O46" s="2"/>
     </row>
     <row r="47" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A47" s="22"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
+      <c r="A47" s="14"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
       <c r="D47" s="3"/>
       <c r="E47" s="6">
         <v>23</v>
@@ -2944,7 +2951,7 @@
       <c r="J47" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="K47" s="12"/>
+      <c r="K47" s="11"/>
       <c r="L47" s="1" t="s">
         <v>102</v>
       </c>
@@ -2957,9 +2964,9 @@
       <c r="O47" s="2"/>
     </row>
     <row r="48" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A48" s="22"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
+      <c r="A48" s="14"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
       <c r="D48" s="3"/>
       <c r="E48" s="6">
         <v>22</v>
@@ -2981,7 +2988,7 @@
       <c r="J48" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="K48" s="12"/>
+      <c r="K48" s="11"/>
       <c r="L48" s="1" t="s">
         <v>102</v>
       </c>
@@ -2994,9 +3001,9 @@
       <c r="O48" s="2"/>
     </row>
     <row r="49" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A49" s="22"/>
-      <c r="B49" s="12"/>
-      <c r="C49" s="12"/>
+      <c r="A49" s="14"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
       <c r="D49" s="2"/>
       <c r="E49" s="6">
         <v>6</v>
@@ -3016,7 +3023,7 @@
       <c r="J49" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K49" s="12"/>
+      <c r="K49" s="11"/>
       <c r="L49" s="1" t="s">
         <v>105</v>
       </c>
@@ -3029,9 +3036,9 @@
       <c r="O49" s="2"/>
     </row>
     <row r="50" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A50" s="22"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
+      <c r="A50" s="14"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
       <c r="D50" s="2"/>
       <c r="E50" s="6">
         <v>5</v>
@@ -3053,7 +3060,7 @@
       <c r="J50" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="K50" s="12"/>
+      <c r="K50" s="11"/>
       <c r="L50" s="1" t="s">
         <v>105</v>
       </c>
@@ -3066,9 +3073,9 @@
       <c r="O50" s="2"/>
     </row>
     <row r="51" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A51" s="22"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
+      <c r="A51" s="14"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
       <c r="D51" s="2"/>
       <c r="E51" s="6">
         <v>3</v>
@@ -3088,7 +3095,7 @@
       <c r="J51" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="K51" s="12"/>
+      <c r="K51" s="11"/>
       <c r="L51" s="1" t="s">
         <v>108</v>
       </c>
@@ -3101,9 +3108,9 @@
       <c r="O51" s="2"/>
     </row>
     <row r="52" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A52" s="22"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
+      <c r="A52" s="14"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
       <c r="D52" s="2"/>
       <c r="E52" s="6">
         <v>2</v>
@@ -3125,7 +3132,7 @@
       <c r="J52" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="K52" s="20"/>
+      <c r="K52" s="12"/>
       <c r="L52" s="1" t="s">
         <v>108</v>
       </c>
@@ -3138,11 +3145,11 @@
       <c r="O52" s="2"/>
     </row>
     <row r="53" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A53" s="22"/>
-      <c r="B53" s="11" t="s">
+      <c r="A53" s="14"/>
+      <c r="B53" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C53" s="10" t="s">
         <v>141</v>
       </c>
       <c r="D53" s="3"/>
@@ -3164,7 +3171,7 @@
       <c r="J53" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="K53" s="11" t="s">
+      <c r="K53" s="10" t="s">
         <v>105</v>
       </c>
       <c r="L53" s="1"/>
@@ -3177,9 +3184,9 @@
       <c r="O53" s="2"/>
     </row>
     <row r="54" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A54" s="22"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
+      <c r="A54" s="14"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
       <c r="D54" s="3"/>
       <c r="E54" s="6">
         <v>25</v>
@@ -3201,7 +3208,7 @@
       <c r="J54" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="K54" s="12"/>
+      <c r="K54" s="11"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1">
         <v>1</v>
@@ -3212,9 +3219,9 @@
       <c r="O54" s="2"/>
     </row>
     <row r="55" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A55" s="22"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
+      <c r="A55" s="14"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
       <c r="D55" s="3"/>
       <c r="E55" s="6">
         <v>23</v>
@@ -3234,7 +3241,7 @@
       <c r="J55" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="K55" s="12"/>
+      <c r="K55" s="11"/>
       <c r="L55" s="1"/>
       <c r="M55" s="1">
         <v>1</v>
@@ -3245,9 +3252,9 @@
       <c r="O55" s="2"/>
     </row>
     <row r="56" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A56" s="22"/>
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
+      <c r="A56" s="14"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
       <c r="D56" s="3"/>
       <c r="E56" s="6">
         <v>22</v>
@@ -3269,7 +3276,7 @@
       <c r="J56" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="K56" s="12"/>
+      <c r="K56" s="11"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1">
         <v>1</v>
@@ -3280,9 +3287,9 @@
       <c r="O56" s="2"/>
     </row>
     <row r="57" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A57" s="22"/>
-      <c r="B57" s="12"/>
-      <c r="C57" s="12"/>
+      <c r="A57" s="14"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
       <c r="D57" s="2"/>
       <c r="E57" s="6">
         <v>6</v>
@@ -3302,7 +3309,7 @@
       <c r="J57" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="K57" s="12"/>
+      <c r="K57" s="11"/>
       <c r="L57" s="1"/>
       <c r="M57" s="1">
         <v>1</v>
@@ -3313,9 +3320,9 @@
       <c r="O57" s="2"/>
     </row>
     <row r="58" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A58" s="22"/>
-      <c r="B58" s="12"/>
-      <c r="C58" s="12"/>
+      <c r="A58" s="14"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
       <c r="D58" s="2"/>
       <c r="E58" s="6">
         <v>5</v>
@@ -3337,7 +3344,7 @@
       <c r="J58" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="K58" s="12"/>
+      <c r="K58" s="11"/>
       <c r="L58" s="1"/>
       <c r="M58" s="1">
         <v>1</v>
@@ -3348,9 +3355,9 @@
       <c r="O58" s="2"/>
     </row>
     <row r="59" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A59" s="22"/>
-      <c r="B59" s="12"/>
-      <c r="C59" s="12"/>
+      <c r="A59" s="14"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
       <c r="D59" s="2"/>
       <c r="E59" s="6">
         <v>3</v>
@@ -3370,7 +3377,7 @@
       <c r="J59" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="K59" s="12"/>
+      <c r="K59" s="11"/>
       <c r="L59" s="1"/>
       <c r="M59" s="1">
         <v>1</v>
@@ -3381,9 +3388,9 @@
       <c r="O59" s="2"/>
     </row>
     <row r="60" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A60" s="22"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="20"/>
+      <c r="A60" s="14"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
       <c r="D60" s="2"/>
       <c r="E60" s="6">
         <v>2</v>
@@ -3405,7 +3412,7 @@
       <c r="J60" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="K60" s="20"/>
+      <c r="K60" s="12"/>
       <c r="L60" s="1"/>
       <c r="M60" s="1">
         <v>1</v>
@@ -3416,11 +3423,11 @@
       <c r="O60" s="2"/>
     </row>
     <row r="61" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A61" s="22"/>
-      <c r="B61" s="11" t="s">
+      <c r="A61" s="14"/>
+      <c r="B61" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C61" s="11" t="s">
+      <c r="C61" s="10" t="s">
         <v>132</v>
       </c>
       <c r="D61" s="3"/>
@@ -3442,7 +3449,7 @@
       <c r="J61" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="K61" s="11" t="s">
+      <c r="K61" s="10" t="s">
         <v>130</v>
       </c>
       <c r="L61" s="1"/>
@@ -3455,9 +3462,9 @@
       <c r="O61" s="2"/>
     </row>
     <row r="62" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A62" s="22"/>
-      <c r="B62" s="12"/>
-      <c r="C62" s="12"/>
+      <c r="A62" s="14"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="11"/>
       <c r="D62" s="3"/>
       <c r="E62" s="6">
         <v>25</v>
@@ -3479,7 +3486,7 @@
       <c r="J62" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="K62" s="12"/>
+      <c r="K62" s="11"/>
       <c r="L62" s="1"/>
       <c r="M62" s="1">
         <v>1</v>
@@ -3490,9 +3497,9 @@
       <c r="O62" s="2"/>
     </row>
     <row r="63" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A63" s="22"/>
-      <c r="B63" s="12"/>
-      <c r="C63" s="12"/>
+      <c r="A63" s="14"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
       <c r="D63" s="3"/>
       <c r="E63" s="6">
         <v>23</v>
@@ -3512,7 +3519,7 @@
       <c r="J63" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="K63" s="12"/>
+      <c r="K63" s="11"/>
       <c r="L63" s="1"/>
       <c r="M63" s="1">
         <v>1</v>
@@ -3523,9 +3530,9 @@
       <c r="O63" s="2"/>
     </row>
     <row r="64" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A64" s="22"/>
-      <c r="B64" s="12"/>
-      <c r="C64" s="12"/>
+      <c r="A64" s="14"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
       <c r="D64" s="3"/>
       <c r="E64" s="6">
         <v>22</v>
@@ -3547,7 +3554,7 @@
       <c r="J64" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="K64" s="12"/>
+      <c r="K64" s="11"/>
       <c r="L64" s="1"/>
       <c r="M64" s="1">
         <v>1</v>
@@ -3558,9 +3565,9 @@
       <c r="O64" s="2"/>
     </row>
     <row r="65" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A65" s="22"/>
-      <c r="B65" s="12"/>
-      <c r="C65" s="12"/>
+      <c r="A65" s="14"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
       <c r="D65" s="2"/>
       <c r="E65" s="6">
         <v>6</v>
@@ -3580,7 +3587,7 @@
       <c r="J65" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="K65" s="12"/>
+      <c r="K65" s="11"/>
       <c r="L65" s="1"/>
       <c r="M65" s="1">
         <v>1</v>
@@ -3591,9 +3598,9 @@
       <c r="O65" s="2"/>
     </row>
     <row r="66" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A66" s="22"/>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
+      <c r="A66" s="14"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
       <c r="D66" s="2"/>
       <c r="E66" s="6">
         <v>5</v>
@@ -3615,7 +3622,7 @@
       <c r="J66" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="K66" s="12"/>
+      <c r="K66" s="11"/>
       <c r="L66" s="1"/>
       <c r="M66" s="1">
         <v>1</v>
@@ -3626,9 +3633,9 @@
       <c r="O66" s="2"/>
     </row>
     <row r="67" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A67" s="22"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="12"/>
+      <c r="A67" s="14"/>
+      <c r="B67" s="11"/>
+      <c r="C67" s="11"/>
       <c r="D67" s="2"/>
       <c r="E67" s="6">
         <v>3</v>
@@ -3648,7 +3655,7 @@
       <c r="J67" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="K67" s="12"/>
+      <c r="K67" s="11"/>
       <c r="L67" s="1"/>
       <c r="M67" s="1">
         <v>1</v>
@@ -3659,9 +3666,9 @@
       <c r="O67" s="2"/>
     </row>
     <row r="68" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A68" s="22"/>
-      <c r="B68" s="20"/>
-      <c r="C68" s="20"/>
+      <c r="A68" s="14"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
       <c r="D68" s="2"/>
       <c r="E68" s="6">
         <v>2</v>
@@ -3683,7 +3690,7 @@
       <c r="J68" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="K68" s="20"/>
+      <c r="K68" s="12"/>
       <c r="L68" s="1"/>
       <c r="M68" s="1">
         <v>1</v>
@@ -3694,11 +3701,11 @@
       <c r="O68" s="2"/>
     </row>
     <row r="69" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A69" s="22"/>
-      <c r="B69" s="11" t="s">
+      <c r="A69" s="14"/>
+      <c r="B69" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C69" s="11" t="s">
+      <c r="C69" s="10" t="s">
         <v>122</v>
       </c>
       <c r="D69" s="3"/>
@@ -3720,7 +3727,7 @@
       <c r="J69" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="K69" s="11" t="s">
+      <c r="K69" s="10" t="s">
         <v>111</v>
       </c>
       <c r="L69" s="1"/>
@@ -3733,9 +3740,9 @@
       <c r="O69" s="2"/>
     </row>
     <row r="70" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A70" s="22"/>
-      <c r="B70" s="12"/>
-      <c r="C70" s="12"/>
+      <c r="A70" s="14"/>
+      <c r="B70" s="11"/>
+      <c r="C70" s="11"/>
       <c r="D70" s="3"/>
       <c r="E70" s="6">
         <v>25</v>
@@ -3757,7 +3764,7 @@
       <c r="J70" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="K70" s="12"/>
+      <c r="K70" s="11"/>
       <c r="L70" s="1"/>
       <c r="M70" s="1">
         <v>1</v>
@@ -3768,9 +3775,9 @@
       <c r="O70" s="2"/>
     </row>
     <row r="71" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A71" s="22"/>
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
+      <c r="A71" s="14"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
       <c r="D71" s="3"/>
       <c r="E71" s="6">
         <v>23</v>
@@ -3790,7 +3797,7 @@
       <c r="J71" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="K71" s="12"/>
+      <c r="K71" s="11"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1">
         <v>1</v>
@@ -3801,9 +3808,9 @@
       <c r="O71" s="2"/>
     </row>
     <row r="72" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A72" s="22"/>
-      <c r="B72" s="12"/>
-      <c r="C72" s="12"/>
+      <c r="A72" s="14"/>
+      <c r="B72" s="11"/>
+      <c r="C72" s="11"/>
       <c r="D72" s="3"/>
       <c r="E72" s="6">
         <v>22</v>
@@ -3825,7 +3832,7 @@
       <c r="J72" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="K72" s="12"/>
+      <c r="K72" s="11"/>
       <c r="L72" s="1"/>
       <c r="M72" s="1">
         <v>1</v>
@@ -3836,9 +3843,9 @@
       <c r="O72" s="2"/>
     </row>
     <row r="73" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A73" s="22"/>
-      <c r="B73" s="12"/>
-      <c r="C73" s="12"/>
+      <c r="A73" s="14"/>
+      <c r="B73" s="11"/>
+      <c r="C73" s="11"/>
       <c r="D73" s="2"/>
       <c r="E73" s="6">
         <v>6</v>
@@ -3858,7 +3865,7 @@
       <c r="J73" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="K73" s="12"/>
+      <c r="K73" s="11"/>
       <c r="L73" s="1"/>
       <c r="M73" s="1">
         <v>1</v>
@@ -3869,9 +3876,9 @@
       <c r="O73" s="2"/>
     </row>
     <row r="74" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A74" s="22"/>
-      <c r="B74" s="12"/>
-      <c r="C74" s="12"/>
+      <c r="A74" s="14"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="11"/>
       <c r="D74" s="2"/>
       <c r="E74" s="6">
         <v>5</v>
@@ -3893,7 +3900,7 @@
       <c r="J74" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="K74" s="12"/>
+      <c r="K74" s="11"/>
       <c r="L74" s="1"/>
       <c r="M74" s="1">
         <v>1</v>
@@ -3904,9 +3911,9 @@
       <c r="O74" s="2"/>
     </row>
     <row r="75" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A75" s="22"/>
-      <c r="B75" s="12"/>
-      <c r="C75" s="12"/>
+      <c r="A75" s="14"/>
+      <c r="B75" s="11"/>
+      <c r="C75" s="11"/>
       <c r="D75" s="2"/>
       <c r="E75" s="6">
         <v>3</v>
@@ -3926,7 +3933,7 @@
       <c r="J75" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="K75" s="12"/>
+      <c r="K75" s="11"/>
       <c r="L75" s="1"/>
       <c r="M75" s="1">
         <v>1</v>
@@ -3937,9 +3944,9 @@
       <c r="O75" s="2"/>
     </row>
     <row r="76" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A76" s="22"/>
-      <c r="B76" s="20"/>
-      <c r="C76" s="20"/>
+      <c r="A76" s="14"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
       <c r="D76" s="2"/>
       <c r="E76" s="6">
         <v>2</v>
@@ -3961,7 +3968,7 @@
       <c r="J76" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="K76" s="20"/>
+      <c r="K76" s="12"/>
       <c r="L76" s="1"/>
       <c r="M76" s="1">
         <v>1</v>
@@ -3973,14 +3980,20 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="A23:A34"/>
-    <mergeCell ref="B23:B34"/>
-    <mergeCell ref="C23:C34"/>
-    <mergeCell ref="K23:K34"/>
-    <mergeCell ref="B35:B44"/>
-    <mergeCell ref="C35:C44"/>
-    <mergeCell ref="K35:K44"/>
-    <mergeCell ref="A35:A76"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="B69:B76"/>
+    <mergeCell ref="C69:C76"/>
+    <mergeCell ref="K69:K76"/>
+    <mergeCell ref="B53:B60"/>
+    <mergeCell ref="C53:C60"/>
+    <mergeCell ref="K53:K60"/>
+    <mergeCell ref="B61:B68"/>
+    <mergeCell ref="C61:C68"/>
+    <mergeCell ref="K61:K68"/>
+    <mergeCell ref="C45:C52"/>
+    <mergeCell ref="K45:K52"/>
+    <mergeCell ref="B45:B52"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
@@ -3997,20 +4010,14 @@
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="B69:B76"/>
-    <mergeCell ref="C69:C76"/>
-    <mergeCell ref="K69:K76"/>
-    <mergeCell ref="B53:B60"/>
-    <mergeCell ref="C53:C60"/>
-    <mergeCell ref="K53:K60"/>
-    <mergeCell ref="B61:B68"/>
-    <mergeCell ref="C61:C68"/>
-    <mergeCell ref="K61:K68"/>
-    <mergeCell ref="C45:C52"/>
-    <mergeCell ref="K45:K52"/>
-    <mergeCell ref="B45:B52"/>
+    <mergeCell ref="A23:A34"/>
+    <mergeCell ref="B23:B34"/>
+    <mergeCell ref="C23:C34"/>
+    <mergeCell ref="K23:K34"/>
+    <mergeCell ref="B35:B44"/>
+    <mergeCell ref="C35:C44"/>
+    <mergeCell ref="K35:K44"/>
+    <mergeCell ref="A35:A76"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="O45:O52 B3:G3 B4:F52 G4:G76 J24:L52 N24:O44 M24:M76 J3:O23">

</xml_diff>